<commit_message>
updated azure login in PS scripts
</commit_message>
<xml_diff>
--- a/AKSResourceCalculation.xlsx
+++ b/AKSResourceCalculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ARCSoftwares\ARCDeliverable\KubernetesResourceCalculationForAKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADA5BA9-64EE-4594-8410-FA00676B31B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22845B60-3ADF-47E1-8959-25ED3132AE9E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8EEBC7D8-CB00-4C0F-ADAC-3223FD186D2E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>AKS Resource Limits</t>
   </si>
@@ -210,12 +210,24 @@
   <si>
     <t>https://stackoverflow.com/questions/52898067/aks-reporting-insufficient-pods</t>
   </si>
+  <si>
+    <t>Pod CPU/Memory requests define a set amount of CPU and memory that the pod needs on a regular basis</t>
+  </si>
+  <si>
+    <t>Pod CPU/Memory limits are the maximum amount of CPU and memory that a pod can use. These limits help define which pods should be killed in the event of node instability due to insufficient resources.</t>
+  </si>
+  <si>
+    <t>it is very important to monitor the performance of your application at different times during the day or week. Determine when the peak demand is, and align the pod limits to the resources required to meet the application's max needs.</t>
+  </si>
+  <si>
+    <t>For this activity to take place we have to deploy and test the entire functioning application so that the deployment files can be changed accordingly for requests and limits.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +247,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -282,17 +301,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -303,12 +316,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -626,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2204C0BE-C50C-46BF-B56A-43C3E6F89F00}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+      <selection activeCell="A10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,347 +659,376 @@
     <col min="1" max="1" width="47.08984375" customWidth="1"/>
     <col min="2" max="2" width="28.54296875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" customWidth="1"/>
     <col min="5" max="5" width="17.81640625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="10" spans="1:8" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D17" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E17" t="s">
         <v>14</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G17" t="s">
         <v>16</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H17" t="s">
         <v>17</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>1</v>
       </c>
-      <c r="B12">
+      <c r="B18">
         <v>1000</v>
       </c>
-      <c r="C12">
+      <c r="C18">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+    <row r="19" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="9" t="s">
+    <row r="31" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
+    <row r="34" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-    </row>
-    <row r="30" spans="1:4" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="9" t="s">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+    </row>
+    <row r="36" spans="1:4" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-    </row>
-    <row r="32" spans="1:4" ht="43" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+    </row>
+    <row r="38" spans="1:4" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-    </row>
-    <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-    </row>
-    <row r="35" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-    </row>
-    <row r="37" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="10" t="s">
+    <row r="41" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-    </row>
-    <row r="43" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="9" t="s">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+    </row>
+    <row r="49" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
+    <row r="52" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="161.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="9" t="s">
+    <row r="53" spans="1:4" ht="161.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="9" t="s">
+    <row r="59" spans="1:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-    </row>
-    <row r="54" spans="1:4" ht="246.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+    </row>
+    <row r="60" spans="1:4" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A50:D50"/>
+  <mergeCells count="16">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A49:D49"/>
     <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A55" r:id="rId1" location="support-for-cooldown-delay" display="https://kubernetes.io/docs/tasks/run-application/horizontal-pod-autoscale/ - support-for-cooldown-delay" xr:uid="{0F79CC2F-AF69-4097-BFCC-5880ADBFF9EA}"/>
-    <hyperlink ref="A36" r:id="rId2" xr:uid="{E9673195-1844-4F9D-AA3C-07C20B24EDB6}"/>
+    <hyperlink ref="A61" r:id="rId1" location="support-for-cooldown-delay" display="https://kubernetes.io/docs/tasks/run-application/horizontal-pod-autoscale/ - support-for-cooldown-delay" xr:uid="{0F79CC2F-AF69-4097-BFCC-5880ADBFF9EA}"/>
+    <hyperlink ref="A42" r:id="rId2" xr:uid="{E9673195-1844-4F9D-AA3C-07C20B24EDB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>

</xml_diff>